<commit_message>
aplicacion funcional al 31jul2025
</commit_message>
<xml_diff>
--- a/data/ejemplo_importacion_productos.xlsx
+++ b/data/ejemplo_importacion_productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\inventario_app2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5659AD8F-1210-4DD3-9998-FD15580B0F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E05EAD-8B7B-4A11-9C29-8E327AB65926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{355AC9BA-97F2-4343-A85C-93DDBF089E10}"/>
+    <workbookView xWindow="-28920" yWindow="-900" windowWidth="29040" windowHeight="16440" xr2:uid="{355AC9BA-97F2-4343-A85C-93DDBF089E10}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -439,10 +439,14 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>